<commit_message>
One of the more final versions
</commit_message>
<xml_diff>
--- a/Final Submission/Model Results.xlsx
+++ b/Final Submission/Model Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E9F0B21F-8B3E-4AE5-A084-11EC3018B4BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F7AE19D7-1142-4EEF-A91E-3AE90A8A99AE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual &amp; Ensemble Model" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Cross Validation'!$B$2:$E$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Individual &amp; Ensemble Model'!$B$2:$D$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Individual &amp; Ensemble Model'!$B$2:$F$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SMOTE-NC'!$B$2:$D$13</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Model</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>K-Nearest Neighbour</t>
+  </si>
+  <si>
+    <t>Train (%)</t>
+  </si>
+  <si>
+    <t>Validation (%)</t>
+  </si>
+  <si>
+    <t>Test (%)</t>
   </si>
 </sst>
 </file>
@@ -460,140 +469,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>72.930000000000007</v>
+      </c>
+      <c r="D3" s="1">
+        <v>72.87</v>
+      </c>
+      <c r="E3" s="1">
+        <v>69.36</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>68.77</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C4" s="1">
+        <v>70.38</v>
+      </c>
+      <c r="D4" s="1">
+        <v>70.03</v>
+      </c>
+      <c r="E4" s="1">
+        <v>67.52</v>
+      </c>
+      <c r="F4" s="1">
         <v>0.73</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>71.11</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>76.98</v>
+      </c>
+      <c r="D5" s="1">
+        <v>79.83</v>
+      </c>
+      <c r="E5" s="1">
+        <v>73.62</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>79.84</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C6" s="1">
+        <v>80.8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>81.39</v>
+      </c>
+      <c r="E6" s="1">
+        <v>78.3</v>
+      </c>
+      <c r="F6" s="1">
         <v>0.71</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>83.3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>79.83</v>
+      </c>
+      <c r="E7" s="1">
+        <v>77.16</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>81.819999999999993</v>
+      </c>
+      <c r="D8" s="1">
+        <v>81.25</v>
+      </c>
+      <c r="E8" s="1">
+        <v>77.45</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1">
+        <v>88.34</v>
+      </c>
+      <c r="D9" s="1">
+        <v>79.12</v>
+      </c>
+      <c r="E9" s="1">
+        <v>76.31</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
-        <v>77.069999999999993</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C10" s="1">
+        <v>99.75</v>
+      </c>
+      <c r="D10" s="1">
+        <v>79.83</v>
+      </c>
+      <c r="E10" s="1">
+        <v>75.040000000000006</v>
+      </c>
+      <c r="F10" s="1">
         <v>0.67</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>79.349999999999994</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
-        <v>72.180000000000007</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C11" s="1">
+        <v>99.75</v>
+      </c>
+      <c r="D11" s="1">
+        <v>75.849999999999994</v>
+      </c>
+      <c r="E11" s="1">
+        <v>70.209999999999994</v>
+      </c>
+      <c r="F11" s="1">
         <v>0.65</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1">
-        <v>74.31</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C12" s="1">
+        <v>83.51</v>
+      </c>
+      <c r="D12" s="1">
+        <v>74.86</v>
+      </c>
+      <c r="E12" s="1">
+        <v>70.209999999999994</v>
+      </c>
+      <c r="F12" s="1">
         <v>0.65</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>78.489999999999995</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>75.37</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>77.72</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.68</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="B2:F12" xr:uid="{1375B292-CAE4-448F-A8C8-3A96A75F8076}">
+    <sortState ref="B3:F12">
+      <sortCondition descending="1" ref="F2:F12"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
The presentation seems to be done v1
</commit_message>
<xml_diff>
--- a/Final Submission/Model Results.xlsx
+++ b/Final Submission/Model Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{406A8CBF-1BB9-4CF5-83AA-D8BCE35AE839}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{13CD7862-9E23-4F13-BD0C-D96890DFAB2B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6030" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual &amp; Ensemble Model" sheetId="1" r:id="rId1"/>
@@ -512,7 +512,7 @@
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,70 +542,70 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>72.930000000000007</v>
+        <v>99.75</v>
       </c>
       <c r="D3" s="1">
-        <v>72.87</v>
+        <v>79.83</v>
       </c>
       <c r="E3" s="1">
-        <v>69.36</v>
+        <v>75.040000000000006</v>
       </c>
       <c r="F3" s="1">
-        <v>0.74</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>70.38</v>
+        <v>99.75</v>
       </c>
       <c r="D4" s="1">
-        <v>70.03</v>
+        <v>75.849999999999994</v>
       </c>
       <c r="E4" s="1">
-        <v>67.52</v>
+        <v>70.209999999999994</v>
       </c>
       <c r="F4" s="1">
-        <v>0.73</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>76.98</v>
+        <v>88.34</v>
       </c>
       <c r="D5" s="1">
-        <v>79.83</v>
+        <v>79.12</v>
       </c>
       <c r="E5" s="1">
-        <v>73.62</v>
+        <v>76.31</v>
       </c>
       <c r="F5" s="1">
-        <v>0.72</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>80.8</v>
+        <v>83.51</v>
       </c>
       <c r="D6" s="1">
-        <v>81.39</v>
+        <v>74.86</v>
       </c>
       <c r="E6" s="1">
-        <v>78.3</v>
+        <v>70.209999999999994</v>
       </c>
       <c r="F6" s="1">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -644,76 +644,76 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>88.34</v>
+        <v>80.8</v>
       </c>
       <c r="D9" s="1">
-        <v>79.12</v>
+        <v>81.39</v>
       </c>
       <c r="E9" s="1">
-        <v>76.31</v>
+        <v>78.3</v>
       </c>
       <c r="F9" s="1">
-        <v>0.68</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
-        <v>99.75</v>
+        <v>76.98</v>
       </c>
       <c r="D10" s="1">
         <v>79.83</v>
       </c>
       <c r="E10" s="1">
-        <v>75.040000000000006</v>
+        <v>73.62</v>
       </c>
       <c r="F10" s="1">
-        <v>0.67</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1">
-        <v>99.75</v>
+        <v>72.930000000000007</v>
       </c>
       <c r="D11" s="1">
-        <v>75.849999999999994</v>
+        <v>72.87</v>
       </c>
       <c r="E11" s="1">
-        <v>70.209999999999994</v>
+        <v>69.36</v>
       </c>
       <c r="F11" s="1">
-        <v>0.65</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
-        <v>83.51</v>
+        <v>70.38</v>
       </c>
       <c r="D12" s="1">
-        <v>74.86</v>
+        <v>70.03</v>
       </c>
       <c r="E12" s="1">
-        <v>70.209999999999994</v>
+        <v>67.52</v>
       </c>
       <c r="F12" s="1">
-        <v>0.65</v>
+        <v>0.73</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B2:F12" xr:uid="{1375B292-CAE4-448F-A8C8-3A96A75F8076}">
     <sortState ref="B3:F12">
-      <sortCondition descending="1" ref="F2:F12"/>
+      <sortCondition descending="1" ref="C2:C12"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -913,7 +913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2B42BF-0C0D-4FD7-AACA-54B07F4DA92F}">
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -937,24 +937,24 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1">
-        <v>75.650000000000006</v>
+        <v>76.959999999999994</v>
       </c>
       <c r="D3" s="1">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1">
-        <v>73.27</v>
+        <v>76.959999999999994</v>
       </c>
       <c r="D4" s="1">
-        <v>0.84</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -981,21 +981,21 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1">
-        <v>75.599999999999994</v>
+        <v>75.650000000000006</v>
       </c>
       <c r="D7" s="1">
-        <v>0.83</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>71.62</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="D8" s="1">
         <v>0.83</v>
@@ -1003,21 +1003,21 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
-        <v>70.02</v>
+        <v>74.23</v>
       </c>
       <c r="D9" s="1">
-        <v>0.83</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1">
-        <v>76.959999999999994</v>
+        <v>73.38</v>
       </c>
       <c r="D10" s="1">
         <v>0.82</v>
@@ -1025,41 +1025,41 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1">
-        <v>73.38</v>
+        <v>73.27</v>
       </c>
       <c r="D11" s="1">
-        <v>0.82</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1">
-        <v>76.959999999999994</v>
+        <v>71.62</v>
       </c>
       <c r="D12" s="1">
-        <v>0.81</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1">
-        <v>74.23</v>
+        <v>70.02</v>
       </c>
       <c r="D13" s="1">
-        <v>0.79</v>
+        <v>0.83</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B2:D13" xr:uid="{727D4B4B-59D4-49DF-9722-5B9DF7E86543}">
     <sortState ref="B3:D13">
-      <sortCondition descending="1" ref="D2:D13"/>
+      <sortCondition descending="1" ref="C2:C13"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1070,7 +1070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0326E2-DAC4-4F6F-BD0F-CC181C0F7079}">
   <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>